<commit_message>
-Updated Binary tree and Linked lists -added unit testing for Linked lists
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S166282\Documents\2018_AIE_Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2408F92D-AFE2-4F99-9022-8970E1CF8073}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7733A421-F369-4F68-9B78-FA84424FE498}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First year" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Second Year" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>Math for Games</t>
   </si>
@@ -206,6 +207,12 @@
   </si>
   <si>
     <t>D:\builds for game jam 2\PC_installer</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Complex Games</t>
   </si>
 </sst>
 </file>
@@ -325,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -644,6 +651,43 @@
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
@@ -660,7 +704,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -724,6 +768,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -731,6 +787,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
@@ -742,34 +816,37 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1063,7 +1140,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:A13"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,10 +1169,10 @@
       <c r="E1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="41"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1108,10 +1185,10 @@
       <c r="E2" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="41"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1120,10 +1197,10 @@
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="17"/>
-      <c r="F3" s="41"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1132,7 +1209,7 @@
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="32"/>
-      <c r="F4" s="41"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24"/>
@@ -1140,10 +1217,10 @@
       <c r="C5" s="25"/>
       <c r="D5" s="7"/>
       <c r="E5" s="23"/>
-      <c r="F5" s="41"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="45" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1154,10 +1231,10 @@
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="30"/>
-      <c r="F6" s="41"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1166,18 +1243,18 @@
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="41"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1190,10 +1267,10 @@
       <c r="E9" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1202,10 +1279,10 @@
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="41"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1214,10 +1291,10 @@
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="17"/>
-      <c r="F11" s="41"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1228,10 +1305,10 @@
       <c r="E12" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
@@ -1240,18 +1317,18 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="41"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1262,10 +1339,10 @@
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="41"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1274,10 +1351,10 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="41"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
@@ -1286,10 +1363,10 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="41"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1298,18 +1375,18 @@
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="29"/>
-      <c r="F18" s="41"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="26" t="s">
@@ -1320,10 +1397,10 @@
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="41"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1332,10 +1409,10 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="41"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="27" t="s">
         <v>23</v>
       </c>
@@ -1344,18 +1421,18 @@
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="41"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="35"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1368,10 +1445,10 @@
         <v>53</v>
       </c>
       <c r="E24" s="30"/>
-      <c r="F24" s="41"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
@@ -1382,10 +1459,10 @@
       <c r="E25" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="41"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1398,10 +1475,10 @@
       <c r="E26" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
@@ -1414,18 +1491,18 @@
       <c r="E27" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="35"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="42" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -1436,10 +1513,10 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="28"/>
-      <c r="F29" s="41"/>
+      <c r="F29" s="35"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="46"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="6" t="s">
         <v>31</v>
       </c>
@@ -1448,10 +1525,10 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="18"/>
-      <c r="F30" s="41"/>
+      <c r="F30" s="35"/>
     </row>
     <row r="31" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="6" t="s">
         <v>32</v>
       </c>
@@ -1460,10 +1537,10 @@
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="41"/>
+      <c r="F31" s="35"/>
     </row>
     <row r="32" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="6" t="s">
         <v>33</v>
       </c>
@@ -1472,10 +1549,10 @@
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="18"/>
-      <c r="F32" s="41"/>
+      <c r="F32" s="35"/>
     </row>
     <row r="33" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="6" t="s">
         <v>34</v>
       </c>
@@ -1484,18 +1561,18 @@
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="41"/>
+      <c r="F33" s="35"/>
     </row>
     <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="35"/>
     </row>
     <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="42" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -1506,10 +1583,10 @@
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="28"/>
-      <c r="F35" s="41"/>
+      <c r="F35" s="35"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="46"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="9" t="s">
         <v>37</v>
       </c>
@@ -1518,10 +1595,10 @@
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="18"/>
-      <c r="F36" s="41"/>
+      <c r="F36" s="35"/>
     </row>
     <row r="37" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="9" t="s">
         <v>38</v>
       </c>
@@ -1530,10 +1607,10 @@
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="18"/>
-      <c r="F37" s="41"/>
+      <c r="F37" s="35"/>
     </row>
     <row r="38" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="47"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="6" t="s">
         <v>39</v>
       </c>
@@ -1544,15 +1621,15 @@
         <v>41</v>
       </c>
       <c r="E38" s="29"/>
-      <c r="F38" s="41"/>
+      <c r="F38" s="35"/>
     </row>
     <row r="39" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="35"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1586,12 +1663,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209D3D92-06A5-4F9D-B0E1-24FC89124B29}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="68.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="16" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:F5"/>
+    <mergeCell ref="A5:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated Checklist status of "Unit Tests for Linked List, Binary Tree, Hash Map" from not started -> current. updated Checklist status of "version control" from not started -> submitted (date included)
Remaining major assessments for first year: 4
Remaining minor assessments for first year: 9
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S166282\Documents\2018_AIE_Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5705FB-F471-44F4-A3DE-C80DE89864A4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115E7C0F-13E7-4753-AA86-9FD70F44DCCB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>Math for Games</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>2018_AIE_Work\1stYear\CodeDesignAndStructures\Assignment\Documentation</t>
+  </si>
+  <si>
+    <t>[Current]</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -484,73 +487,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="7" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="7" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -843,19 +849,19 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24:E27"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="54.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -877,565 +883,566 @@
       <c r="F1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="D2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="10"/>
+      <c r="D3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="10"/>
+      <c r="D4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
+      <c r="D9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="10"/>
+      <c r="C10" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="17">
+        <v>43231</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="10"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="10"/>
+      <c r="D15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="10"/>
+      <c r="D17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="10"/>
+      <c r="D18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="10"/>
+      <c r="D20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="10"/>
+      <c r="D21" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="10"/>
+      <c r="D22" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="10"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="17">
         <v>43229</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="10"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="17">
         <v>43231</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="10"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="17">
         <v>43229</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="25" t="s">
+      <c r="E26" s="12"/>
+      <c r="F26" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="10"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="17">
         <v>43229</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="25" t="s">
+      <c r="E27" s="12"/>
+      <c r="F27" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="10"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="10"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="10"/>
+      <c r="D29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="10"/>
+      <c r="D30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="10"/>
+      <c r="D31" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="10"/>
+      <c r="D32" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="10"/>
+      <c r="D33" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="10"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="10"/>
+      <c r="D35" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="10"/>
+      <c r="D36" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="10"/>
+      <c r="D37" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="26" t="s">
+      <c r="D38" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="10"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:A4"/>
     <mergeCell ref="G1:G39"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A8:F8"/>
@@ -1452,7 +1459,6 @@
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E38" r:id="rId1" xr:uid="{68008070-7FDE-470F-8996-55DFB5C0BF57}"/>
@@ -1478,7 +1484,7 @@
     <col min="1" max="1" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" style="8" customWidth="1"/>
@@ -1504,47 +1510,47 @@
       <c r="F1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="11"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="28"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D6"/>

</xml_diff>

<commit_message>
Updated Checklist to contain second year assessments which have not been reviewed, and are not yet colour coded. Updated debugging as completed (as it will be completed as i continue to complete all the assessments) Updated good coding practices as completed (as it will be completed as i continue to complete all the assessments)
Minor Assessments remaining: 5
Major Assessments remaining: 4
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S166282\Documents\2018_AIE_Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s166282\Desktop\AIE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115E7C0F-13E7-4753-AA86-9FD70F44DCCB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4CC45B-8DC2-4127-ADCB-8F7346505FA9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
   <si>
     <t>Math for Games</t>
   </si>
@@ -218,6 +218,60 @@
   </si>
   <si>
     <t>[Current]</t>
+  </si>
+  <si>
+    <t>Computer Graphics</t>
+  </si>
+  <si>
+    <t>Modular Complex System document</t>
+  </si>
+  <si>
+    <t>modular system</t>
+  </si>
+  <si>
+    <t>Source code and assets for the system submitted</t>
+  </si>
+  <si>
+    <t>review doc</t>
+  </si>
+  <si>
+    <t>can run external to an IDE without errors</t>
+  </si>
+  <si>
+    <t>Implementation of static and dynamic rigid body physics that interact together</t>
+  </si>
+  <si>
+    <t>Forces applied to physics bodies</t>
+  </si>
+  <si>
+    <t>Visualisation of physics bodies</t>
+  </si>
+  <si>
+    <t>Physics simulations run as expected without physical errors</t>
+  </si>
+  <si>
+    <t>Creation of class diagrams for the Custom Physics Simulation</t>
+  </si>
+  <si>
+    <t>Physics System’s classes, their properties, relationships and how they interact together</t>
+  </si>
+  <si>
+    <t>Physics Joints</t>
+  </si>
+  <si>
+    <t>Ragdoll Physics</t>
+  </si>
+  <si>
+    <t>Raycast into simulation's scene for picking purposes</t>
+  </si>
+  <si>
+    <t>Trigger systems with callback functions that impact the simulation in a meaningful way</t>
+  </si>
+  <si>
+    <t>Use of Character Controller physics bodies supporting dynamic and kinematic rigid bodies</t>
+  </si>
+  <si>
+    <t>Particle Systems that make use of colliders for physical interactions</t>
   </si>
 </sst>
 </file>
@@ -329,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -396,43 +450,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -449,11 +466,57 @@
     </border>
     <border>
       <left/>
-      <right style="double">
+      <right/>
+      <top style="double">
         <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -467,7 +530,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -518,13 +581,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,26 +608,38 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -847,9 +930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,13 +966,13 @@
       <c r="F1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="25"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -902,11 +985,11 @@
       <c r="F2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -917,11 +1000,11 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="26"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -932,19 +1015,19 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="26"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -958,10 +1041,10 @@
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="26"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -973,22 +1056,22 @@
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="26"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1001,14 +1084,14 @@
       <c r="F9" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -1016,10 +1099,10 @@
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1031,10 +1114,10 @@
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="26"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1048,10 +1131,10 @@
       <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1065,19 +1148,19 @@
         <v>62</v>
       </c>
       <c r="F13" s="12"/>
-      <c r="G13" s="26"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1091,10 +1174,10 @@
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="26"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1106,10 +1189,10 @@
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="26"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1121,10 +1204,10 @@
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="26"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1136,19 +1219,19 @@
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="26"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1162,10 +1245,10 @@
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="26"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1177,10 +1260,10 @@
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="26"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1192,19 +1275,19 @@
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="26"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1218,10 +1301,10 @@
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="26"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
@@ -1235,10 +1318,10 @@
       <c r="F25" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="26"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
@@ -1252,10 +1335,10 @@
       <c r="F26" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="26"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1269,19 +1352,19 @@
       <c r="F27" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="26"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="30" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1295,10 +1378,10 @@
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
-      <c r="G29" s="26"/>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
@@ -1310,10 +1393,10 @@
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
-      <c r="G30" s="26"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
@@ -1325,10 +1408,10 @@
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="26"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
@@ -1340,10 +1423,10 @@
       </c>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="26"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
@@ -1355,19 +1438,19 @@
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="26"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1381,10 +1464,10 @@
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="26"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="6" t="s">
         <v>37</v>
       </c>
@@ -1396,10 +1479,10 @@
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="26"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="6" t="s">
         <v>38</v>
       </c>
@@ -1411,10 +1494,10 @@
       </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="26"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="4" t="s">
         <v>39</v>
       </c>
@@ -1428,20 +1511,21 @@
         <v>41</v>
       </c>
       <c r="F38" s="16"/>
-      <c r="G38" s="26"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="G1:G39"/>
     <mergeCell ref="A5:F5"/>
@@ -1458,7 +1542,6 @@
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E38" r:id="rId1" xr:uid="{68008070-7FDE-470F-8996-55DFB5C0BF57}"/>
@@ -1472,18 +1555,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209D3D92-06A5-4F9D-B0E1-24FC89124B29}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="8" bestFit="1" customWidth="1"/>
@@ -1492,174 +1575,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="G1" s="33"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
+      <c r="D2" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="32"/>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="33"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="11"/>
+      <c r="G2" s="34"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="39"/>
+      <c r="B3" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="24" t="s">
+        <v>72</v>
+      </c>
       <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="D4" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D6"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
+      <c r="B12" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D29"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D31"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D32"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="37"/>
+      <c r="B18" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="34"/>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="8"/>
     </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G1:G5"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A3:F3"/>
+  <mergeCells count="5">
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A2:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Checklist to contain unit test checklist for year 1
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s166282\Desktop\AIE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4CC45B-8DC2-4127-ADCB-8F7346505FA9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85108DBD-BF4F-4D23-B734-C955CCA589E8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First year" sheetId="1" r:id="rId1"/>
-    <sheet name="Second Year" sheetId="2" r:id="rId2"/>
+    <sheet name="unit test checklist" sheetId="3" r:id="rId2"/>
+    <sheet name="Second Year" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="99">
   <si>
     <t>Math for Games</t>
   </si>
@@ -272,6 +273,57 @@
   </si>
   <si>
     <t>Particle Systems that make use of colliders for physical interactions</t>
+  </si>
+  <si>
+    <t>Linked list</t>
+  </si>
+  <si>
+    <t>create list</t>
+  </si>
+  <si>
+    <t>pushback</t>
+  </si>
+  <si>
+    <t>push front</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>erase</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>popBack</t>
+  </si>
+  <si>
+    <t>popFront</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -930,9 +982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +993,7 @@
     <col min="2" max="2" width="95.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" style="9" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
@@ -1554,6 +1606,144 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C61E2B-27E6-423E-9BE9-5EDC04A727A5}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209D3D92-06A5-4F9D-B0E1-24FC89124B29}">
   <dimension ref="A1:G53"/>
   <sheetViews>

</xml_diff>

<commit_message>
Split linked list, binary tree and hashmap completion into seperate tasks Completed Linked List (marked off in Unit Checklist book) Completed Linked List Unit Testing
Remaining major assessments for first year: 4
Remaining minor assessments for first year: 9
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s166282\Desktop\AIE Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S166282\Desktop\AIE_Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FC2F5B-90D4-43CF-8BF1-5BDB1488FA3A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7289C434-6B9C-4097-A294-A93393D1DD5C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First year" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
   <si>
     <t>Math for Games</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Hash Map</t>
   </si>
   <si>
-    <t>Unit Tests for Linked List, Binary Tree, Hash Map</t>
-  </si>
-  <si>
     <t>Evidence of Version control</t>
   </si>
   <si>
@@ -348,6 +345,18 @@
   </si>
   <si>
     <t>Gizmo's</t>
+  </si>
+  <si>
+    <t>linked List</t>
+  </si>
+  <si>
+    <t>Unit test for Linked List</t>
+  </si>
+  <si>
+    <t>unit test for Hash Map</t>
+  </si>
+  <si>
+    <t>Unit test for Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -522,21 +531,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,6 +615,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -632,7 +687,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -684,9 +739,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
@@ -695,7 +747,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
@@ -713,6 +765,18 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -722,37 +786,49 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,11 +1118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,598 +1145,648 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="32"/>
+        <v>46</v>
+      </c>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="33"/>
+        <v>49</v>
+      </c>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="33"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="33"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="33"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>60</v>
+      <c r="A9" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="17">
+        <v>43238</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="33"/>
+        <v>47</v>
+      </c>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>60</v>
+      <c r="A10" s="51"/>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="17">
+        <v>43238</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="33"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="17">
-        <v>43231</v>
-      </c>
+      <c r="A11" s="51"/>
+      <c r="B11" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="33"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="51"/>
+      <c r="B12" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="36"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="36"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="36"/>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="17">
+        <v>43231</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="36"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="52"/>
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="C17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="33"/>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="5" t="s">
+      <c r="E17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="36"/>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="33"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="33"/>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
-      <c r="B16" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="33"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="4" t="s">
+      <c r="C19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="36"/>
+    </row>
+    <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37"/>
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
-      <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="33"/>
-    </row>
-    <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-    </row>
-    <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>43</v>
+      <c r="C20" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="33"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30"/>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>43</v>
+      <c r="A21" s="37"/>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="33"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>44</v>
+      <c r="A22" s="37"/>
+      <c r="B22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="33"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="36"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="33"/>
+      <c r="B25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="33"/>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="36"/>
+    </row>
+    <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+    </row>
+    <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="17">
+        <v>43229</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="36"/>
+    </row>
+    <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="37"/>
+      <c r="B29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="17">
+        <v>43231</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="36"/>
+    </row>
+    <row r="30" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="37"/>
+      <c r="B30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="17">
+        <v>43229</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="36"/>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="37"/>
+      <c r="B31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="17">
+        <v>43229</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="36"/>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+    </row>
+    <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="17">
-        <v>43229</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="33"/>
-    </row>
-    <row r="25" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="34"/>
-      <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="17">
-        <v>43231</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="33"/>
-    </row>
-    <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34"/>
-      <c r="B26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="17">
-        <v>43229</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
-      <c r="B27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="17">
-        <v>43229</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="33"/>
-    </row>
-    <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+      <c r="B33" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="33"/>
-    </row>
-    <row r="30" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="33"/>
-    </row>
-    <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="33"/>
-    </row>
-    <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
-      <c r="B32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="33"/>
-    </row>
-    <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="34"/>
-      <c r="B33" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="C33" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="33"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
-        <v>35</v>
-      </c>
+      <c r="A35" s="37"/>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="33"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34"/>
-      <c r="B36" s="6" t="s">
-        <v>37</v>
+      <c r="A36" s="37"/>
+      <c r="B36" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="33"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="34"/>
-      <c r="B37" s="6" t="s">
-        <v>38</v>
+      <c r="A37" s="37"/>
+      <c r="B37" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="33"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="34"/>
-      <c r="B38" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="19" t="s">
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+    </row>
+    <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="16"/>
-      <c r="G38" s="33"/>
-    </row>
-    <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="32"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D39" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="36"/>
+    </row>
+    <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="37"/>
+      <c r="B40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="36"/>
+    </row>
+    <row r="41" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="37"/>
+      <c r="B41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="36"/>
+    </row>
+    <row r="42" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="37"/>
+      <c r="B42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="16"/>
+      <c r="G42" s="36"/>
+    </row>
+    <row r="43" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="48"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="35"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A9:A17"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="G1:G39"/>
+    <mergeCell ref="G1:G43"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A18:F18"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A39:A42"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E38" r:id="rId1" xr:uid="{68008070-7FDE-470F-8996-55DFB5C0BF57}"/>
+    <hyperlink ref="E42" r:id="rId1" xr:uid="{68008070-7FDE-470F-8996-55DFB5C0BF57}"/>
     <hyperlink ref="F9" r:id="rId2" xr:uid="{BF267DB3-CC59-4E22-BA42-CDA9B5F41AB7}"/>
-    <hyperlink ref="F26" r:id="rId3" xr:uid="{4C150602-347B-4EB8-A524-21E0DFFF30E4}"/>
+    <hyperlink ref="F30" r:id="rId3" xr:uid="{4C150602-347B-4EB8-A524-21E0DFFF30E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -1672,7 +1798,7 @@
   <dimension ref="A1:AC46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,153 +1810,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39">
-        <v>2017</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="C2" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="39"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="24" t="s">
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="24" t="s">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="24" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="23" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="24" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
@@ -1932,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209D3D92-06A5-4F9D-B0E1-24FC89124B29}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
@@ -1950,409 +2076,409 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="26"/>
+      <c r="C1" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>70</v>
+      <c r="A2" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="27"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="24" t="s">
-        <v>71</v>
+      <c r="A3" s="45"/>
+      <c r="B3" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="27"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="24" t="s">
-        <v>72</v>
+      <c r="A4" s="45"/>
+      <c r="B4" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="27"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="24" t="s">
-        <v>73</v>
+      <c r="A5" s="45"/>
+      <c r="B5" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="27"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>75</v>
-      </c>
       <c r="D6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="27"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="24" t="s">
-        <v>76</v>
+      <c r="A7" s="45"/>
+      <c r="B7" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="27"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="24" t="s">
-        <v>77</v>
+      <c r="A8" s="45"/>
+      <c r="B8" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="27"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="24" t="s">
-        <v>78</v>
+      <c r="A9" s="45"/>
+      <c r="B9" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="27"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="24" t="s">
-        <v>79</v>
+      <c r="A10" s="45"/>
+      <c r="B10" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="27"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="24" t="s">
-        <v>80</v>
+      <c r="A11" s="45"/>
+      <c r="B11" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="27"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="24" t="s">
-        <v>81</v>
+      <c r="A12" s="46"/>
+      <c r="B12" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="27"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="27"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>65</v>
+      <c r="A14" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="27"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="24" t="s">
-        <v>66</v>
+      <c r="A15" s="39"/>
+      <c r="B15" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="27"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="24" t="s">
-        <v>67</v>
+      <c r="A16" s="39"/>
+      <c r="B16" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="27"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="24" t="s">
-        <v>68</v>
+      <c r="A17" s="39"/>
+      <c r="B17" s="23" t="s">
+        <v>67</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="27"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="24" t="s">
-        <v>69</v>
+      <c r="A18" s="43"/>
+      <c r="B18" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="27"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="27"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>64</v>
+      <c r="A20" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="27"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="45"/>
+      <c r="C21" s="32"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="27"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="20"/>
-      <c r="C22" s="45"/>
+      <c r="C22" s="32"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
-      <c r="G22" s="27"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="45"/>
+      <c r="C23" s="32"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="27"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="32"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
-      <c r="G24" s="27"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="32"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="27"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="45"/>
+      <c r="C26" s="32"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
-      <c r="G26" s="27"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="45"/>
+      <c r="C27" s="32"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="27"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="45"/>
+      <c r="C28" s="32"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="27"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="45"/>
+      <c r="C29" s="32"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="27"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="45"/>
+      <c r="C30" s="32"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="27"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="45"/>
+      <c r="C31" s="32"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="27"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="45"/>
+      <c r="C32" s="32"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="27"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="45"/>
+      <c r="C33" s="32"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
-      <c r="G33" s="27"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="45"/>
+      <c r="C34" s="32"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
-      <c r="G34" s="27"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="45"/>
+      <c r="C35" s="32"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="27"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="45"/>
+      <c r="C36" s="32"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="27"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="27"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D38" s="8"/>

</xml_diff>

<commit_message>
Updated Checklist for MathforGames Binary Math
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S166282\Desktop\AIE_Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s166282\Desktop\AIE WORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7289C434-6B9C-4097-A294-A93393D1DD5C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C58C128-9736-49B3-A676-44FD2590190F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
   <si>
     <t>Math for Games</t>
   </si>
@@ -687,7 +687,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -771,6 +771,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,52 +798,43 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1122,7 +1128,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,10 +1162,10 @@
       <c r="F1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="35"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1175,10 +1181,10 @@
       <c r="F2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="36"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="28" t="s">
         <v>5</v>
       </c>
@@ -1190,10 +1196,10 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="36"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
@@ -1205,36 +1211,36 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="36"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>58</v>
+      <c r="D6" s="54">
+        <v>43283</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="36"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1246,19 +1252,19 @@
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="36"/>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1274,10 +1280,10 @@
       <c r="F9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="36"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>107</v>
       </c>
@@ -1289,10 +1295,10 @@
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="36"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="22" t="s">
         <v>96</v>
       </c>
@@ -1302,10 +1308,10 @@
       <c r="D11" s="13"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="36"/>
+      <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="22" t="s">
         <v>109</v>
       </c>
@@ -1315,10 +1321,10 @@
       <c r="D12" s="13"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1326,10 +1332,10 @@
       <c r="D13" s="13"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="36"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="1" t="s">
         <v>108</v>
       </c>
@@ -1339,10 +1345,10 @@
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="36"/>
+      <c r="G14" s="41"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
@@ -1354,10 +1360,10 @@
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="36"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1371,10 +1377,10 @@
       <c r="F16" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="41"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
@@ -1388,19 +1394,19 @@
         <v>61</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="36"/>
+      <c r="G17" s="41"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1414,10 +1420,10 @@
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="36"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1429,10 +1435,10 @@
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="36"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="4" t="s">
         <v>15</v>
       </c>
@@ -1444,10 +1450,10 @@
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="36"/>
+      <c r="G21" s="41"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
@@ -1459,19 +1465,19 @@
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="36"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1485,10 +1491,10 @@
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="36"/>
+      <c r="G24" s="41"/>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="33"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1500,10 +1506,10 @@
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="36"/>
+      <c r="G25" s="41"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
@@ -1515,19 +1521,19 @@
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="36"/>
+      <c r="G26" s="41"/>
     </row>
     <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="48"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="34" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1541,10 +1547,10 @@
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
-      <c r="G28" s="36"/>
+      <c r="G28" s="41"/>
     </row>
     <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="5" t="s">
         <v>24</v>
       </c>
@@ -1558,10 +1564,10 @@
       <c r="F29" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="36"/>
+      <c r="G29" s="41"/>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="5" t="s">
         <v>25</v>
       </c>
@@ -1575,10 +1581,10 @@
       <c r="F30" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="36"/>
+      <c r="G30" s="41"/>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="5" t="s">
         <v>26</v>
       </c>
@@ -1592,19 +1598,19 @@
       <c r="F31" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="41"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="48"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="34" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1618,10 +1624,10 @@
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="36"/>
+      <c r="G33" s="41"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="4" t="s">
         <v>30</v>
       </c>
@@ -1633,10 +1639,10 @@
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="36"/>
+      <c r="G34" s="41"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="4" t="s">
         <v>31</v>
       </c>
@@ -1648,10 +1654,10 @@
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="36"/>
+      <c r="G35" s="41"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="4" t="s">
         <v>32</v>
       </c>
@@ -1663,10 +1669,10 @@
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="36"/>
+      <c r="G36" s="41"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="4" t="s">
         <v>33</v>
       </c>
@@ -1678,19 +1684,19 @@
       </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="36"/>
+      <c r="G37" s="41"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="48"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -1704,10 +1710,10 @@
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="36"/>
+      <c r="G39" s="41"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="6" t="s">
         <v>36</v>
       </c>
@@ -1719,10 +1725,10 @@
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="36"/>
+      <c r="G40" s="41"/>
     </row>
     <row r="41" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="6" t="s">
         <v>37</v>
       </c>
@@ -1734,10 +1740,10 @@
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="36"/>
+      <c r="G41" s="41"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="37"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="4" t="s">
         <v>38</v>
       </c>
@@ -1751,20 +1757,21 @@
         <v>40</v>
       </c>
       <c r="F42" s="16"/>
-      <c r="G42" s="36"/>
+      <c r="G42" s="41"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="48"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="35"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="40"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A39:A42"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A9:A17"/>
     <mergeCell ref="A6:A7"/>
@@ -1781,7 +1788,6 @@
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A33:A37"/>
-    <mergeCell ref="A39:A42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E42" r:id="rId1" xr:uid="{68008070-7FDE-470F-8996-55DFB5C0BF57}"/>
@@ -1821,10 +1827,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
+      <c r="A2" s="48">
         <v>2017</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="44" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1832,106 +1838,106 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="47"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="47"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="47"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="38" t="s">
+      <c r="A17" s="46"/>
+      <c r="B17" s="45" t="s">
         <v>96</v>
       </c>
       <c r="C17" s="23" t="s">
@@ -1939,22 +1945,22 @@
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="23" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="23" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="23" t="s">
         <v>104</v>
       </c>
@@ -2097,7 +2103,7 @@
       <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="51" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -2112,7 +2118,7 @@
       <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="52"/>
       <c r="B3" s="23" t="s">
         <v>70</v>
       </c>
@@ -2125,7 +2131,7 @@
       <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="23" t="s">
         <v>71</v>
       </c>
@@ -2138,7 +2144,7 @@
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="23" t="s">
         <v>72</v>
       </c>
@@ -2151,7 +2157,7 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="23" t="s">
         <v>73</v>
       </c>
@@ -2166,7 +2172,7 @@
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="23" t="s">
         <v>75</v>
       </c>
@@ -2179,7 +2185,7 @@
       <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="23" t="s">
         <v>76</v>
       </c>
@@ -2192,7 +2198,7 @@
       <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="23" t="s">
         <v>77</v>
       </c>
@@ -2205,7 +2211,7 @@
       <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="23" t="s">
         <v>78</v>
       </c>
@@ -2218,7 +2224,7 @@
       <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="23" t="s">
         <v>79</v>
       </c>
@@ -2231,7 +2237,7 @@
       <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="23" t="s">
         <v>80</v>
       </c>
@@ -2244,16 +2250,16 @@
       <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="48" t="s">
         <v>56</v>
       </c>
       <c r="B14" s="23" t="s">
@@ -2268,7 +2274,7 @@
       <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="23" t="s">
         <v>65</v>
       </c>
@@ -2281,7 +2287,7 @@
       <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="23" t="s">
         <v>66</v>
       </c>
@@ -2294,7 +2300,7 @@
       <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="23" t="s">
         <v>67</v>
       </c>
@@ -2307,7 +2313,7 @@
       <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="23" t="s">
         <v>68</v>
       </c>
@@ -2320,12 +2326,12 @@
       <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2472,12 +2478,12 @@
       <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
       <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Checklist as 03/07/2018
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s166282\Desktop\AIE WORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C58C128-9736-49B3-A676-44FD2590190F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE59EA6-23EF-4DA3-9632-0457A5549310}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
   <si>
     <t>Math for Games</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Will be signed off as we go</t>
   </si>
   <si>
-    <t>Started.</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -357,6 +354,21 @@
   </si>
   <si>
     <t>Unit test for Binary Tree</t>
+  </si>
+  <si>
+    <t>2018_AIE_Work\1stYear</t>
+  </si>
+  <si>
+    <t>2018_AIE_Work\1stYear\Intro to C++\Binary Files</t>
+  </si>
+  <si>
+    <t>2018_AIE_Work\1stYear\MathForGames</t>
+  </si>
+  <si>
+    <t>C:\Users\s166282\Desktop\AIE WORK\1stYear\CodeDesignAndStructures\Assignment\SourceCode\AssessableTutorials\LinkedList</t>
+  </si>
+  <si>
+    <t>(Cross platform app on matts computer)</t>
   </si>
 </sst>
 </file>
@@ -468,7 +480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -676,6 +688,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -687,7 +712,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -708,9 +733,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -753,12 +775,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,30 +784,22 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,6 +812,24 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -822,6 +848,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,7 +863,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1126,18 +1155,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="78.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="128.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" style="9" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
@@ -1154,627 +1183,645 @@
         <v>39</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="40"/>
+        <v>45</v>
+      </c>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="41"/>
+      <c r="C2" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="16">
+        <v>43284</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="28" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="41"/>
+      <c r="D3" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="41"/>
+      <c r="D4" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="41"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="54">
+      <c r="C6" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="16">
         <v>43283</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="41"/>
+      <c r="E6" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="41"/>
+      <c r="D7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="16">
+        <v>43238</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="36"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="42"/>
+      <c r="B10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C10" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D10" s="16">
         <v>43238</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="17">
-        <v>43238</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="41"/>
+      <c r="E10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="41"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="41"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="41"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="41"/>
+        <v>107</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>43231</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="41"/>
+      <c r="E15" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="41"/>
+      <c r="D16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="41"/>
+      <c r="D17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="41"/>
+      <c r="D19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="41"/>
+      <c r="D20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="41"/>
+      <c r="D21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="41"/>
+      <c r="D22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="41"/>
+      <c r="D24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="41"/>
+      <c r="D25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="39"/>
+      <c r="B26" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="41"/>
+      <c r="D26" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="40" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="17">
+      <c r="C28" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="16">
         <v>43229</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="41"/>
+      <c r="E28" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="17">
+      <c r="C29" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="16">
         <v>43231</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="41"/>
+      <c r="E29" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="17">
+      <c r="C30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="16">
         <v>43229</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="41"/>
+      <c r="E30" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="17">
+      <c r="C31" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="16">
         <v>43229</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="41"/>
+      <c r="E31" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="41"/>
+      <c r="D33" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="34"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="41"/>
+      <c r="D34" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="41"/>
+      <c r="D35" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="41"/>
+      <c r="D36" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="34"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="41"/>
+      <c r="D37" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="40" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="41"/>
+      <c r="D39" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="34"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="41"/>
+      <c r="D40" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="34"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="41"/>
+      <c r="D41" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="34"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="19" t="s">
+      <c r="D42" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="41"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="42"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="40"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="35"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="G1:G43"/>
     <mergeCell ref="A5:F5"/>
@@ -1788,14 +1835,19 @@
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E42" r:id="rId1" xr:uid="{68008070-7FDE-470F-8996-55DFB5C0BF57}"/>
     <hyperlink ref="F9" r:id="rId2" xr:uid="{BF267DB3-CC59-4E22-BA42-CDA9B5F41AB7}"/>
     <hyperlink ref="F30" r:id="rId3" xr:uid="{4C150602-347B-4EB8-A524-21E0DFFF30E4}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{809A02E1-80B8-470A-8A6C-C6ED15626EAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1816,159 +1868,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
-        <v>2017</v>
-      </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="47"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="47"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="47"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="23" t="s">
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="23" t="s">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="23" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="23" t="s">
-        <v>104</v>
-      </c>
-    </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="AA31"/>
@@ -2066,7 +2118,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2126,7 @@
     <col min="1" max="1" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" style="8" customWidth="1"/>
@@ -2082,409 +2134,457 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="25"/>
+      <c r="D1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
+      <c r="B8" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="54"/>
+      <c r="B9" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="54"/>
+      <c r="B10" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="55"/>
+      <c r="B12" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="26"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53"/>
-      <c r="B12" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="26"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="23" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="26"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="23" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="26"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="23" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="52"/>
+      <c r="B18" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="26"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="26"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="26"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="26"/>
+      <c r="A20" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="32"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="26"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="32"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="26"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="32"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="26"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="32"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="26"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="32"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="26"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="32"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="26"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="32"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="26"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="32"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="26"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="32"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="26"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="32"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="26"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="32"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="26"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="32"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="26"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="32"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="26"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="32"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="26"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="32"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="26"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="32"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="26"/>
-    </row>
-    <row r="37" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="49"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="26"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="25"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="25"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="51"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D38" s="8"/>

</xml_diff>